<commit_message>
there's a bunch of odd files in the folder; added to a "wtf" folder
</commit_message>
<xml_diff>
--- a/Citeline_CataractDrug.xlsx
+++ b/Citeline_CataractDrug.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -17077,7 +17077,7 @@
   <dimension ref="A1:BI52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>